<commit_message>
Added Different Password Combinations in Excel File for DDT
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8791F84-BD4F-4716-8C37-DAA37C8E529D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EF9E09-1E5E-424F-BA3E-A33FB5188280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="17630" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +47,33 @@
   </si>
   <si>
     <t>EnterPassword1234</t>
+  </si>
+  <si>
+    <t>Wrong Passwords</t>
+  </si>
+  <si>
+    <t>Lowercase</t>
+  </si>
+  <si>
+    <t>a1234</t>
+  </si>
+  <si>
+    <t>Capital and Minimum 8 Characters</t>
+  </si>
+  <si>
+    <t>@@@</t>
+  </si>
+  <si>
+    <t>Not Satisfy any rule</t>
+  </si>
+  <si>
+    <t>Not satisfy</t>
+  </si>
+  <si>
+    <t>Expected Color</t>
+  </si>
+  <si>
+    <t>rgba(255, 0, 0, 1)</t>
   </si>
 </sst>
 </file>
@@ -72,8 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,32 +395,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" customWidth="1"/>
     <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338893DC-7041-483A-B8B7-2D9BD70B2C11}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Update profile scripts
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -3,39 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EF9E09-1E5E-424F-BA3E-A33FB5188280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0A5CA771-77C9-47C5-A0D3-BF29C2205DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="17630" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19460" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -74,6 +61,24 @@
   </si>
   <si>
     <t>rgba(255, 0, 0, 1)</t>
+  </si>
+  <si>
+    <t>Expeceted Title</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Rj</t>
+  </si>
+  <si>
+    <t>Rutu</t>
+  </si>
+  <si>
+    <t>Jadhav</t>
   </si>
 </sst>
 </file>
@@ -395,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,7 +415,7 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +428,11 @@
       <c r="D1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -437,8 +445,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -446,12 +457,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit to merge files
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EF9E09-1E5E-424F-BA3E-A33FB5188280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FA221-9159-4485-9DE9-3A7456B63F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="17630" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="1900" windowWidth="16020" windowHeight="6420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -74,6 +74,33 @@
   </si>
   <si>
     <t>rgba(255, 0, 0, 1)</t>
+  </si>
+  <si>
+    <t>prati23</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>pratibha</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>wabale</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>confirm pass</t>
+  </si>
+  <si>
+    <t>mobileno</t>
+  </si>
+  <si>
+    <t>EnterPassword@1234</t>
   </si>
 </sst>
 </file>
@@ -395,22 +422,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" customWidth="1"/>
     <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -438,7 +467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -446,12 +475,58 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>6754902280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the test case for Change Password Functionality
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Persistent\Projects\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FA221-9159-4485-9DE9-3A7456B63F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1900" windowWidth="16020" windowHeight="6420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="1905" windowWidth="16020" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -101,12 +100,24 @@
   </si>
   <si>
     <t>EnterPassword@1234</t>
+  </si>
+  <si>
+    <t>Function_Change_Password</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>jkl1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,25 +432,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6328125" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -467,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -475,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -483,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -506,7 +517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -527,6 +538,33 @@
       </c>
       <c r="H7">
         <v>6754902280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -535,24 +573,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338893DC-7041-483A-B8B7-2D9BD70B2C11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added more data in excel file
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3FA725-C542-4845-BB5A-5C785113653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27FC3B2-203E-44D1-B59A-B01D9EB752C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>http://test-monk.in/profile</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>jkl1</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,6 +549,17 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed user registration data
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratibha_wabale\git\Mini_Project_Team6\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA55E394-C1D1-49B1-A9CE-40E175E112E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5265694A-2378-44E6-9959-85C5CF0D5BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1716" yWindow="5880" windowWidth="20520" windowHeight="11856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -128,35 +128,50 @@
     <t>Login to iDrive</t>
   </si>
   <si>
-    <t>temp09</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>lasttemp</t>
-  </si>
-  <si>
-    <t>temp@gmail.com</t>
-  </si>
-  <si>
-    <t>Tem@p123</t>
-  </si>
-  <si>
     <t>Tooltip ExpectedText</t>
   </si>
   <si>
     <t>Please include an '@' in the email address. 'prati23' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>pr23</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>wb</t>
+  </si>
+  <si>
+    <t>pr23@gmail.com</t>
+  </si>
+  <si>
+    <t>Password@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,17 +194,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,18 +492,18 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6328125" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -513,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -521,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -529,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -552,7 +570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -575,17 +593,17 @@
         <v>6754902280</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -605,18 +623,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338893DC-7041-483A-B8B7-2D9BD70B2C11}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.90625" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="57.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -627,7 +645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -638,14 +656,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -657,22 +675,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F3AD7C-8B63-4B65-AF58-02708C8106B1}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,30 +713,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>34</v>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="H2" s="1">
         <v>8787878787</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{71746744-B2F0-40DC-B221-78A62228E79C}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{6BED3C38-933F-4743-B7C5-4F260E247458}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rutuja Added test case for update profile
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Mini_Project_Team6\Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5265694A-2378-44E6-9959-85C5CF0D5BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{10DE8923-83C5-49B3-A960-A46BB5B881FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1716" yWindow="5880" windowWidth="20520" windowHeight="11856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="19460" windowHeight="11060" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Registration_Details" sheetId="3" r:id="rId3"/>
+    <sheet name="TestData-Rutuja" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -147,6 +144,27 @@
   </si>
   <si>
     <t>Password@1234</t>
+  </si>
+  <si>
+    <t>utuja</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Rj</t>
+  </si>
+  <si>
+    <t>Rutu</t>
+  </si>
+  <si>
+    <t>Jadhav</t>
+  </si>
+  <si>
+    <t>Rutuja</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -488,22 +506,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -531,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -539,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -547,7 +565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -570,7 +588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -593,17 +611,17 @@
         <v>6754902280</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -627,14 +645,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -645,7 +663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -656,12 +674,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -675,22 +693,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F3AD7C-8B63-4B65-AF58-02708C8106B1}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -744,4 +762,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7ECA9F5-435C-4750-BBBF-4DC2AC6BA9C6}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rutuja made change in excel sheet, pom, excel utils
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutuja_jadhav3\AppData\Local\Programs\Git\Mini_Project_Team6\Mini_Project_Team6\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14BA35-D957-427E-BC04-EB5FD3A2071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="18876" windowHeight="4644" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="15010" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,21 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>username</t>
   </si>
@@ -181,13 +178,73 @@
   </si>
   <si>
     <t>qwpo@gmail.com</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>UpdatePic</t>
+  </si>
+  <si>
+    <t>ChangePassword</t>
+  </si>
+  <si>
+    <t>uploadPage</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/register</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/login</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/dashboard</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/changepassword</t>
+  </si>
+  <si>
+    <t>SignUp</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/upload</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/updateprofile</t>
+  </si>
+  <si>
+    <t>http://test-monk.in/changepic</t>
+  </si>
+  <si>
+    <t>UpdateProfile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +263,12 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -243,6 +306,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,29 +581,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -658,18 +723,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -710,25 +775,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -751,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -774,7 +839,7 @@
         <v>8787878787</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -799,10 +864,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -810,51 +875,167 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="34.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
       </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{A0B01D45-D3A4-48D0-84E0-CB9B730A85C2}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{6746C6F3-0B04-4F0C-A7D8-708F91B78568}"/>
+    <hyperlink ref="E14" r:id="rId4" xr:uid="{9A3E4A90-D34D-41AB-A8B6-D45DF6B01AC8}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{478E3E37-85BA-4A24-B9DB-AEDE6D17AB30}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{1943B8A6-00F0-464A-8139-D9C637556170}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{B1A862BC-3A5E-41C7-B2B8-4E1CDFE60A62}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{D53CFD7D-7F4C-4D67-8EC7-8E6FA1FDEFAE}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{050CD6EE-734E-4C8E-9256-91653B9D310C}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{DF826DB2-A274-4D5C-98B1-C48E45950F1D}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{47D955A8-B73F-4F46-A32C-14331669404F}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{3AB6E32C-A769-4379-A039-C9D7954FFAE4}"/>
+    <hyperlink ref="E13" r:id="rId13" xr:uid="{F2D318F6-9809-4D79-A9CD-35872C9B9B7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ankita Login credentials in User credentials
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutuja_jadhav3\AppData\Local\Programs\Git\Mini_Project_Team6\Mini_Project_Team6\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini_project\Project\Mini_Project_Team6\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14BA35-D957-427E-BC04-EB5FD3A2071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACF8377-E250-4263-9D7D-FD18FB92EA4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="15010" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Registration_Details" sheetId="3" r:id="rId3"/>
     <sheet name="TestData-Rutuja" sheetId="4" r:id="rId4"/>
+    <sheet name="TestData-Ankita" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>username</t>
   </si>
@@ -238,6 +239,27 @@
   </si>
   <si>
     <t>UpdateProfile</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Passward</t>
+  </si>
+  <si>
+    <t>Invalid_Username</t>
+  </si>
+  <si>
+    <t>ankita</t>
+  </si>
+  <si>
+    <t>Pass9Test</t>
+  </si>
+  <si>
+    <t>ankita987</t>
+  </si>
+  <si>
+    <t>Invalid_Password</t>
   </si>
 </sst>
 </file>
@@ -595,18 +617,18 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6328125" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -634,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -642,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -650,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -673,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -696,17 +718,17 @@
         <v>6754902280</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -730,14 +752,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.90625" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="57.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -748,7 +770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -759,12 +781,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -782,18 +804,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -839,7 +861,7 @@
         <v>8787878787</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -878,17 +900,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="34.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -902,7 +924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>51</v>
       </c>
@@ -910,7 +932,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>52</v>
       </c>
@@ -918,7 +940,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>53</v>
       </c>
@@ -926,7 +948,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>57</v>
       </c>
@@ -934,7 +956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -948,7 +970,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -957,7 +979,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -971,7 +993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>69</v>
       </c>
@@ -979,7 +1001,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>55</v>
       </c>
@@ -987,7 +1009,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>56</v>
       </c>
@@ -995,7 +1017,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>53</v>
       </c>
@@ -1003,7 +1025,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>59</v>
       </c>
@@ -1011,7 +1033,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>65</v>
       </c>
@@ -1038,4 +1060,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392653D0-B943-4F5F-9B0D-43AC3B01C75D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dhanashree- modified excel file
</commit_message>
<xml_diff>
--- a/Files/User_Credentials.xlsx
+++ b/Files/User_Credentials.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project\Mini_Project_Team6\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1197EA-C5CF-4DD2-B379-472793068005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="17496" windowHeight="6744" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>username</t>
   </si>
@@ -268,12 +274,15 @@
   </si>
   <si>
     <t>Dhanu@000</t>
+  </si>
+  <si>
+    <t>WrongMobile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,32 +620,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B19" activeCellId="1" sqref="A19 B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -664,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -672,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -680,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -703,7 +712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -726,17 +735,17 @@
         <v>6754902280</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -747,7 +756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
     </row>
   </sheetData>
@@ -756,18 +765,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -808,25 +817,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -849,7 +858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -872,7 +881,7 @@
         <v>8787878787</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.95" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -897,10 +906,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -908,17 +917,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="34.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1054,19 +1063,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E14" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="E9" r:id="rId9"/>
-    <hyperlink ref="E10" r:id="rId10"/>
-    <hyperlink ref="E11" r:id="rId11"/>
-    <hyperlink ref="E12" r:id="rId12"/>
-    <hyperlink ref="E13" r:id="rId13"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E14" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="E13" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -1074,19 +1083,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1123,23 +1132,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="8.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="2" max="4" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1174,11 @@
       <c r="H1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.95" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1187,8 +1200,11 @@
       <c r="H3">
         <v>1231231230</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>859476574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1196,7 +1212,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1207,32 +1223,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.95" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>1231231230</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1291,9 +1307,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>